<commit_message>
updated WM 2018 excel file
</commit_message>
<xml_diff>
--- a/src/main/resources/excelimport/WM2018.xlsx
+++ b/src/main/resources/excelimport/WM2018.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="273">
   <si>
     <t>Country 1</t>
   </si>
@@ -749,6 +749,102 @@
   </si>
   <si>
     <t>Moskau</t>
+  </si>
+  <si>
+    <t>Sieger C</t>
+  </si>
+  <si>
+    <t>Zweiter D</t>
+  </si>
+  <si>
+    <t>Sieger A</t>
+  </si>
+  <si>
+    <t>Zweiter B</t>
+  </si>
+  <si>
+    <t>Sieger B</t>
+  </si>
+  <si>
+    <t>Zweiter A</t>
+  </si>
+  <si>
+    <t>Sieger D</t>
+  </si>
+  <si>
+    <t>Zweiter C</t>
+  </si>
+  <si>
+    <t>Sieger E</t>
+  </si>
+  <si>
+    <t>Zweiter F</t>
+  </si>
+  <si>
+    <t>Sieger G</t>
+  </si>
+  <si>
+    <t>Zweiter H</t>
+  </si>
+  <si>
+    <t>Sieger F</t>
+  </si>
+  <si>
+    <t>Sieger H</t>
+  </si>
+  <si>
+    <t>Zweiter E</t>
+  </si>
+  <si>
+    <t>Zweiter G</t>
+  </si>
+  <si>
+    <t>Sieger A1</t>
+  </si>
+  <si>
+    <t>Zweiter A2</t>
+  </si>
+  <si>
+    <t>Sieger A3</t>
+  </si>
+  <si>
+    <t>Zweiter A4</t>
+  </si>
+  <si>
+    <t>Sieger A5</t>
+  </si>
+  <si>
+    <t>Zweiter A6</t>
+  </si>
+  <si>
+    <t>Sieger A7</t>
+  </si>
+  <si>
+    <t>Zweiter A8</t>
+  </si>
+  <si>
+    <t>Sieger HF1</t>
+  </si>
+  <si>
+    <t>Sieger HF2</t>
+  </si>
+  <si>
+    <t>Verlierer HF1</t>
+  </si>
+  <si>
+    <t>Verlierer HF2</t>
+  </si>
+  <si>
+    <t>Sieger VF1</t>
+  </si>
+  <si>
+    <t>Sieger VF2</t>
+  </si>
+  <si>
+    <t>Sieger VF4</t>
+  </si>
+  <si>
+    <t>Sieger VF3</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1214,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E440"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1963,96 +2061,320 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D50" s="2"/>
+      <c r="A50" t="s">
+        <v>241</v>
+      </c>
+      <c r="B50" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" s="2">
+        <v>43281.666666666664</v>
+      </c>
+      <c r="E50" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="2"/>
+      <c r="A51" t="s">
+        <v>243</v>
+      </c>
+      <c r="B51" t="s">
+        <v>244</v>
+      </c>
+      <c r="C51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D51" s="2">
+        <v>43281.833333333336</v>
+      </c>
+      <c r="E51" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="2"/>
+      <c r="A52" t="s">
+        <v>245</v>
+      </c>
+      <c r="B52" t="s">
+        <v>246</v>
+      </c>
+      <c r="C52" t="s">
+        <v>223</v>
+      </c>
+      <c r="D52" s="2">
+        <v>43282.75</v>
+      </c>
+      <c r="E52" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D53" s="2"/>
+      <c r="A53" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" t="s">
+        <v>248</v>
+      </c>
+      <c r="C53" t="s">
+        <v>223</v>
+      </c>
+      <c r="D53" s="2">
+        <v>43282.833333333336</v>
+      </c>
+      <c r="E53" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D54" s="2"/>
+      <c r="A54" t="s">
+        <v>249</v>
+      </c>
+      <c r="B54" t="s">
+        <v>250</v>
+      </c>
+      <c r="C54" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" s="2">
+        <v>43283.666666666664</v>
+      </c>
+      <c r="E54" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D55" s="2"/>
+      <c r="A55" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" t="s">
+        <v>252</v>
+      </c>
+      <c r="C55" t="s">
+        <v>223</v>
+      </c>
+      <c r="D55" s="2">
+        <v>43283.833333333336</v>
+      </c>
+      <c r="E55" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D56" s="2"/>
+      <c r="A56" t="s">
+        <v>253</v>
+      </c>
+      <c r="B56" t="s">
+        <v>255</v>
+      </c>
+      <c r="C56" t="s">
+        <v>223</v>
+      </c>
+      <c r="D56" s="2">
+        <v>43284.666666666664</v>
+      </c>
+      <c r="E56" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D57" s="2"/>
+      <c r="A57" t="s">
+        <v>254</v>
+      </c>
+      <c r="B57" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" t="s">
+        <v>223</v>
+      </c>
+      <c r="D57" s="2">
+        <v>43284.833333333336</v>
+      </c>
+      <c r="E57" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D58" s="2"/>
+      <c r="A58" t="s">
+        <v>257</v>
+      </c>
+      <c r="B58" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="2">
+        <v>43287.666666666664</v>
+      </c>
+      <c r="E58" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D59" s="2"/>
+      <c r="A59" t="s">
+        <v>259</v>
+      </c>
+      <c r="B59" t="s">
+        <v>260</v>
+      </c>
+      <c r="C59" t="s">
+        <v>224</v>
+      </c>
+      <c r="D59" s="2">
+        <v>43288.833333333336</v>
+      </c>
+      <c r="E59" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D60" s="2"/>
+      <c r="A60" t="s">
+        <v>261</v>
+      </c>
+      <c r="B60" t="s">
+        <v>262</v>
+      </c>
+      <c r="C60" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="2">
+        <v>43287.833333333336</v>
+      </c>
+      <c r="E60" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D61" s="2"/>
+      <c r="A61" t="s">
+        <v>263</v>
+      </c>
+      <c r="B61" t="s">
+        <v>264</v>
+      </c>
+      <c r="C61" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" s="2">
+        <v>43288.666666666664</v>
+      </c>
+      <c r="E61" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D62" s="2"/>
+      <c r="A62" t="s">
+        <v>270</v>
+      </c>
+      <c r="B62" t="s">
+        <v>269</v>
+      </c>
+      <c r="C62" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="2">
+        <v>43291.833333333336</v>
+      </c>
+      <c r="E62" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D63" s="2"/>
+      <c r="A63" t="s">
+        <v>271</v>
+      </c>
+      <c r="B63" t="s">
+        <v>272</v>
+      </c>
+      <c r="C63" t="s">
+        <v>225</v>
+      </c>
+      <c r="D63" s="2">
+        <v>43292.833333333336</v>
+      </c>
+      <c r="E63" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>265</v>
+      </c>
+      <c r="B64" t="s">
+        <v>266</v>
+      </c>
+      <c r="C64" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="2">
+        <v>43296.708333333336</v>
+      </c>
+      <c r="E64" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>267</v>
+      </c>
+      <c r="B65" t="s">
+        <v>268</v>
+      </c>
+      <c r="C65" t="s">
+        <v>227</v>
+      </c>
+      <c r="D65" s="2">
+        <v>43295.666666666664</v>
+      </c>
+      <c r="E65" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>